<commit_message>
Updated Mikolaj test plan
</commit_message>
<xml_diff>
--- a/Sprint 2/Test_Driven_Development/Sprint 2 Test Plan.xlsx
+++ b/Sprint 2/Test_Driven_Development/Sprint 2 Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\Novadapt\XAMPP\htdocs\AC31007\Sprint 2\Test_Driven_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ED871F-9354-4B39-8628-91CC14A149C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7265ED01-F7F9-4419-8AEB-2A0D4B17090B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E217C390-6FB7-4EA9-915E-5405BF097C0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>As a Lab Manager/Head Researcher, I need the ability to manage all other users in a system so that I can manage their accounts. #81</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Jordan</t>
+  </si>
+  <si>
+    <t>Mikolaj</t>
   </si>
 </sst>
 </file>
@@ -508,11 +511,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -520,13 +523,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,15 +586,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,19 +602,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4185,8 +4188,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4208,11 +4211,11 @@
       <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:29" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="4" t="s">
@@ -4261,8 +4264,8 @@
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -4297,7 +4300,7 @@
         <v>45</v>
       </c>
       <c r="D5" s="19"/>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F5" s="1"/>
@@ -4334,7 +4337,7 @@
         <v>46</v>
       </c>
       <c r="D6" s="19"/>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F6" s="1"/>
@@ -4371,7 +4374,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="1"/>
@@ -4408,7 +4411,7 @@
         <v>48</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F8" s="1"/>
@@ -4445,7 +4448,7 @@
         <v>49</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="1"/>
@@ -4482,7 +4485,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F10" s="1"/>
@@ -4519,7 +4522,7 @@
         <v>51</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F11" s="1"/>
@@ -4553,8 +4556,8 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -4796,8 +4799,8 @@
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -4969,8 +4972,8 @@
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -5005,7 +5008,9 @@
         <v>21</v>
       </c>
       <c r="D25" s="19"/>
-      <c r="E25" s="18"/>
+      <c r="E25" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -5040,7 +5045,9 @@
         <v>22</v>
       </c>
       <c r="D26" s="19"/>
-      <c r="E26" s="18"/>
+      <c r="E26" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -5075,7 +5082,9 @@
         <v>23</v>
       </c>
       <c r="D27" s="19"/>
-      <c r="E27" s="18"/>
+      <c r="E27" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -5110,7 +5119,9 @@
         <v>24</v>
       </c>
       <c r="D28" s="19"/>
-      <c r="E28" s="18"/>
+      <c r="E28" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -5142,8 +5153,8 @@
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -5178,7 +5189,9 @@
         <v>25</v>
       </c>
       <c r="D30" s="19"/>
-      <c r="E30" s="18"/>
+      <c r="E30" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -5213,7 +5226,9 @@
         <v>26</v>
       </c>
       <c r="D31" s="19"/>
-      <c r="E31" s="18"/>
+      <c r="E31" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -5248,7 +5263,9 @@
         <v>27</v>
       </c>
       <c r="D32" s="19"/>
-      <c r="E32" s="18"/>
+      <c r="E32" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -5280,8 +5297,8 @@
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -5418,8 +5435,8 @@
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -5454,7 +5471,7 @@
         <v>31</v>
       </c>
       <c r="D38" s="19"/>
-      <c r="E38" s="28" t="s">
+      <c r="E38" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F38" s="1"/>
@@ -5491,7 +5508,7 @@
         <v>32</v>
       </c>
       <c r="D39" s="19"/>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F39" s="1"/>
@@ -5528,7 +5545,7 @@
         <v>33</v>
       </c>
       <c r="D40" s="19"/>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F40" s="1"/>
@@ -5562,8 +5579,8 @@
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -5598,7 +5615,7 @@
         <v>34</v>
       </c>
       <c r="D42" s="19"/>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F42" s="1"/>
@@ -5635,7 +5652,7 @@
         <v>35</v>
       </c>
       <c r="D43" s="19"/>
-      <c r="E43" s="28" t="s">
+      <c r="E43" s="22" t="s">
         <v>53</v>
       </c>
       <c r="F43" s="1"/>
@@ -5669,8 +5686,8 @@
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
     </row>
     <row r="45" spans="1:29" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
@@ -5681,7 +5698,7 @@
         <v>40</v>
       </c>
       <c r="D45" s="19"/>
-      <c r="E45" s="28" t="s">
+      <c r="E45" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5694,7 +5711,7 @@
         <v>41</v>
       </c>
       <c r="D46" s="19"/>
-      <c r="E46" s="28" t="s">
+      <c r="E46" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5707,7 +5724,7 @@
         <v>42</v>
       </c>
       <c r="D47" s="19"/>
-      <c r="E47" s="28" t="s">
+      <c r="E47" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5720,7 +5737,7 @@
         <v>43</v>
       </c>
       <c r="D48" s="19"/>
-      <c r="E48" s="28" t="s">
+      <c r="E48" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5730,8 +5747,8 @@
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
@@ -5742,7 +5759,7 @@
         <v>44</v>
       </c>
       <c r="D50" s="19"/>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="22" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5784,6 +5801,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="D49:E49"/>
@@ -5792,9 +5812,6 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sprint 2 test plan updated
</commit_message>
<xml_diff>
--- a/Sprint 2/Test_Driven_Development/Sprint 2 Test Plan.xlsx
+++ b/Sprint 2/Test_Driven_Development/Sprint 2 Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\Novadapt\XAMPP\htdocs\AC31007\Sprint 2\Test_Driven_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7265ED01-F7F9-4419-8AEB-2A0D4B17090B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221727AF-D315-4E4B-BD20-02C960D02B99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E217C390-6FB7-4EA9-915E-5405BF097C0A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>As a Lab Manager/Head Researcher, I need the ability to manage all other users in a system so that I can manage their accounts. #81</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>do you have the abilty to change a researcher's details?</t>
-  </si>
-  <si>
-    <t>do you have the ability to have an interface which operates this?</t>
   </si>
   <si>
     <t>do you have the abiliy to create a specific researcher view?</t>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>Mikolaj</t>
+  </si>
+  <si>
+    <t>Do you have a user interface that allows this to be done?</t>
+  </si>
+  <si>
+    <t>Not Working</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -470,34 +473,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="4" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -514,9 +510,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,6 +524,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -558,15 +581,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -618,15 +641,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,15 +713,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4188,50 +4211,50 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="30" customWidth="1"/>
     <col min="3" max="3" width="54.5703125" customWidth="1"/>
     <col min="4" max="4" width="59.85546875" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" spans="1:29" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:29" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
+      <c r="B3" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>52</v>
+      <c r="E3" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -4259,13 +4282,13 @@
       <c r="AC3" s="1"/>
     </row>
     <row r="4" spans="1:29" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -4292,16 +4315,16 @@
       <c r="AC4" s="1"/>
     </row>
     <row r="5" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="8">
+      <c r="A5" s="11"/>
+      <c r="B5" s="24">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="22" t="s">
-        <v>53</v>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -4329,16 +4352,16 @@
       <c r="AC5" s="1"/>
     </row>
     <row r="6" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="8">
+      <c r="A6" s="11"/>
+      <c r="B6" s="24">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="22" t="s">
-        <v>53</v>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -4366,16 +4389,16 @@
       <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="8">
+      <c r="A7" s="11"/>
+      <c r="B7" s="24">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="22" t="s">
-        <v>53</v>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -4403,16 +4426,16 @@
       <c r="AC7" s="1"/>
     </row>
     <row r="8" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="8">
+      <c r="A8" s="11"/>
+      <c r="B8" s="24">
         <v>4</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22" t="s">
-        <v>53</v>
+      <c r="C8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -4440,16 +4463,16 @@
       <c r="AC8" s="1"/>
     </row>
     <row r="9" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="8">
+      <c r="A9" s="11"/>
+      <c r="B9" s="24">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="22" t="s">
-        <v>53</v>
+      <c r="C9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4477,16 +4500,16 @@
       <c r="AC9" s="1"/>
     </row>
     <row r="10" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="8">
+      <c r="A10" s="11"/>
+      <c r="B10" s="24">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22" t="s">
-        <v>53</v>
+      <c r="C10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -4514,16 +4537,16 @@
       <c r="AC10" s="1"/>
     </row>
     <row r="11" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="8">
+      <c r="A11" s="11"/>
+      <c r="B11" s="24">
         <v>7</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22" t="s">
-        <v>53</v>
+      <c r="C11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -4551,13 +4574,13 @@
       <c r="AC11" s="1"/>
     </row>
     <row r="12" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -4584,15 +4607,17 @@
       <c r="AC12" s="1"/>
     </row>
     <row r="13" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="8">
+      <c r="A13" s="11"/>
+      <c r="B13" s="24">
         <v>8</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -4619,15 +4644,17 @@
       <c r="AC13" s="1"/>
     </row>
     <row r="14" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="8">
+      <c r="A14" s="11"/>
+      <c r="B14" s="24">
         <v>9</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -4654,15 +4681,17 @@
       <c r="AC14" s="1"/>
     </row>
     <row r="15" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="8">
+      <c r="A15" s="11"/>
+      <c r="B15" s="24">
         <v>10</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -4689,15 +4718,17 @@
       <c r="AC15" s="1"/>
     </row>
     <row r="16" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="8">
+      <c r="A16" s="11"/>
+      <c r="B16" s="24">
         <v>11</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -4724,15 +4755,17 @@
       <c r="AC16" s="1"/>
     </row>
     <row r="17" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="8">
+      <c r="A17" s="11"/>
+      <c r="B17" s="24">
         <v>12</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -4759,15 +4792,17 @@
       <c r="AC17" s="1"/>
     </row>
     <row r="18" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="8">
+      <c r="A18" s="11"/>
+      <c r="B18" s="24">
         <v>13</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="18"/>
+      <c r="C18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="15" t="s">
+        <v>52</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -4794,13 +4829,13 @@
       <c r="AC18" s="1"/>
     </row>
     <row r="19" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -4827,15 +4862,17 @@
       <c r="AC19" s="1"/>
     </row>
     <row r="20" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="8">
+      <c r="A20" s="11"/>
+      <c r="B20" s="24">
         <v>14</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="18"/>
+      <c r="C20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -4862,15 +4899,17 @@
       <c r="AC20" s="1"/>
     </row>
     <row r="21" spans="1:29" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="8">
+      <c r="A21" s="11"/>
+      <c r="B21" s="24">
         <v>15</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18"/>
+      <c r="C21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -4897,15 +4936,17 @@
       <c r="AC21" s="1"/>
     </row>
     <row r="22" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="8">
+      <c r="A22" s="11"/>
+      <c r="B22" s="24">
         <v>16</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="18"/>
+      <c r="C22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -4932,15 +4973,17 @@
       <c r="AC22" s="1"/>
     </row>
     <row r="23" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="8">
+      <c r="A23" s="11"/>
+      <c r="B23" s="24">
         <v>17</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="18"/>
+      <c r="C23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -4967,13 +5010,13 @@
       <c r="AC23" s="1"/>
     </row>
     <row r="24" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -5000,16 +5043,16 @@
       <c r="AC24" s="1"/>
     </row>
     <row r="25" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="8">
+      <c r="A25" s="11"/>
+      <c r="B25" s="24">
         <v>18</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="22" t="s">
-        <v>54</v>
+      <c r="C25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -5037,16 +5080,16 @@
       <c r="AC25" s="1"/>
     </row>
     <row r="26" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="8">
+      <c r="A26" s="11"/>
+      <c r="B26" s="24">
         <v>19</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="22" t="s">
-        <v>54</v>
+      <c r="C26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -5074,16 +5117,16 @@
       <c r="AC26" s="1"/>
     </row>
     <row r="27" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="8">
+      <c r="A27" s="11"/>
+      <c r="B27" s="24">
         <v>20</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="22" t="s">
-        <v>54</v>
+      <c r="C27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -5111,16 +5154,16 @@
       <c r="AC27" s="1"/>
     </row>
     <row r="28" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="8">
+      <c r="A28" s="11"/>
+      <c r="B28" s="24">
         <v>21</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="22" t="s">
-        <v>54</v>
+      <c r="C28" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -5148,13 +5191,13 @@
       <c r="AC28" s="1"/>
     </row>
     <row r="29" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -5181,16 +5224,16 @@
       <c r="AC29" s="1"/>
     </row>
     <row r="30" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="8">
+      <c r="A30" s="11"/>
+      <c r="B30" s="24">
         <v>22</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="22" t="s">
-        <v>54</v>
+      <c r="C30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -5218,16 +5261,16 @@
       <c r="AC30" s="1"/>
     </row>
     <row r="31" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="8">
+      <c r="A31" s="11"/>
+      <c r="B31" s="24">
         <v>23</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="22" t="s">
-        <v>54</v>
+      <c r="C31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="12"/>
+      <c r="E31" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -5255,16 +5298,16 @@
       <c r="AC31" s="1"/>
     </row>
     <row r="32" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="8">
+      <c r="A32" s="11"/>
+      <c r="B32" s="24">
         <v>24</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="19"/>
-      <c r="E32" s="22" t="s">
-        <v>54</v>
+      <c r="C32" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -5292,13 +5335,13 @@
       <c r="AC32" s="1"/>
     </row>
     <row r="33" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -5325,15 +5368,17 @@
       <c r="AC33" s="1"/>
     </row>
     <row r="34" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="8">
+      <c r="A34" s="11"/>
+      <c r="B34" s="24">
         <v>25</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="19"/>
-      <c r="E34" s="18"/>
+      <c r="C34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -5360,15 +5405,17 @@
       <c r="AC34" s="1"/>
     </row>
     <row r="35" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="8">
+      <c r="A35" s="11"/>
+      <c r="B35" s="24">
         <v>26</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="18"/>
+      <c r="C35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -5395,15 +5442,17 @@
       <c r="AC35" s="1"/>
     </row>
     <row r="36" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="8">
+      <c r="A36" s="11"/>
+      <c r="B36" s="24">
         <v>27</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="18"/>
+      <c r="C36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="15" t="s">
+        <v>53</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -5430,13 +5479,13 @@
       <c r="AC36" s="1"/>
     </row>
     <row r="37" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -5463,16 +5512,16 @@
       <c r="AC37" s="1"/>
     </row>
     <row r="38" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="8">
+      <c r="A38" s="11"/>
+      <c r="B38" s="24">
         <v>28</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="22" t="s">
-        <v>53</v>
+      <c r="C38" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -5500,16 +5549,16 @@
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="8">
+      <c r="A39" s="11"/>
+      <c r="B39" s="24">
         <v>29</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="22" t="s">
-        <v>53</v>
+      <c r="C39" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -5537,16 +5586,16 @@
       <c r="AC39" s="1"/>
     </row>
     <row r="40" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="8">
+      <c r="A40" s="11"/>
+      <c r="B40" s="24">
         <v>30</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="22" t="s">
-        <v>53</v>
+      <c r="C40" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -5574,13 +5623,13 @@
       <c r="AC40" s="1"/>
     </row>
     <row r="41" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -5607,16 +5656,16 @@
       <c r="AC41" s="1"/>
     </row>
     <row r="42" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="10">
+      <c r="A42" s="11"/>
+      <c r="B42" s="26">
         <v>31</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="22" t="s">
-        <v>53</v>
+      <c r="C42" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -5644,16 +5693,16 @@
       <c r="AC42" s="1"/>
     </row>
     <row r="43" spans="1:29" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="10">
+      <c r="A43" s="11"/>
+      <c r="B43" s="26">
         <v>32</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="22" t="s">
-        <v>53</v>
+      <c r="C43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -5681,137 +5730,137 @@
       <c r="AC43" s="1"/>
     </row>
     <row r="44" spans="1:29" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
+      <c r="A44" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="25"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
     </row>
     <row r="45" spans="1:29" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="10">
+      <c r="A45" s="11"/>
+      <c r="B45" s="26">
         <v>33</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="22" t="s">
-        <v>53</v>
+      <c r="C45" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="10">
+      <c r="A46" s="11"/>
+      <c r="B46" s="26">
         <v>34</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="22" t="s">
-        <v>53</v>
+      <c r="C46" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
-      <c r="B47" s="10">
+      <c r="A47" s="11"/>
+      <c r="B47" s="26">
         <v>35</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="22" t="s">
-        <v>53</v>
+      <c r="C47" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="10">
+      <c r="A48" s="11"/>
+      <c r="B48" s="26">
         <v>36</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="22" t="s">
-        <v>53</v>
+      <c r="C48" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
+      <c r="A49" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="25"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
     </row>
     <row r="50" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="10">
+      <c r="A50" s="11"/>
+      <c r="B50" s="26">
         <v>37</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="22" t="s">
-        <v>53</v>
+      <c r="C50" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D44:E44"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>